<commit_message>
about to remove DL from preprocessor
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_totalseg.xlsx
+++ b/configurations/experiment_configs_totalseg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="128">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -402,9 +402,6 @@
   </si>
   <si>
     <t xml:space="preserve">plan1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lits,drli,litq,litqsmall</t>
   </si>
   <si>
     <t xml:space="preserve">1.5, 1.5,1.5</t>
@@ -659,7 +656,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1016,8 +1013,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1270,7 +1267,7 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1520,7 +1517,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1656,7 +1653,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1767,7 +1764,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1880,8 +1877,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2006,10 +2003,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2038,9 +2035,7 @@
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2057,7 +2052,7 @@
         <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2088,7 +2083,7 @@
         <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2096,7 +2091,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2</v>
@@ -2110,7 +2105,21 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>96</v>
+      </c>
       <c r="E10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
config parser unified out_channel identification and other fixes
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_totalseg.xlsx
+++ b/configurations/experiment_configs_totalseg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -17,6 +17,7 @@
     <sheet name="plan2" sheetId="7" state="visible" r:id="rId9"/>
     <sheet name="plan3" sheetId="8" state="visible" r:id="rId10"/>
     <sheet name="plan4" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="plan5" sheetId="10" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="130">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -412,6 +413,12 @@
   </si>
   <si>
     <t xml:space="preserve">1,1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSL.all,TSL.label_minimal</t>
   </si>
 </sst>
 </file>
@@ -1007,6 +1014,149 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.9"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1014,8 +1164,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1148,12 +1298,12 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="0"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>56</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="0"/>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -1229,7 +1379,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="8"/>
       <c r="E14" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1243,7 +1393,7 @@
         <v>64</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>65</v>
@@ -2146,10 +2296,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2242,25 +2392,30 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1"/>
+      <c r="A9" s="0" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B12" s="1" t="n">
         <v>96</v>
       </c>
     </row>

</xml_diff>